<commit_message>
Add/Edit/Delete Product (first commit)
</commit_message>
<xml_diff>
--- a/MyShop/MyShop/data.xlsx
+++ b/MyShop/MyShop/data.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbxmi\source\repos\PagingExcel\PagingExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbxmi\OneDrive\Documents\MyShop\MyShop\MyShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E142B7D3-EC8B-4BC9-93E4-6BE79DF55050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EECAFF-8DC9-4EE3-9E40-CD6A83729D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{A807BC73-C3E1-4A21-B5F0-B1391A1E9092}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A807BC73-C3E1-4A21-B5F0-B1391A1E9092}"/>
   </bookViews>
   <sheets>
-    <sheet name="Asus" sheetId="1" r:id="rId1"/>
-    <sheet name="Dell" sheetId="2" r:id="rId2"/>
-    <sheet name="Apple" sheetId="3" r:id="rId3"/>
+    <sheet name="HP" sheetId="1" r:id="rId1"/>
+    <sheet name="MSI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>STT</t>
   </si>
@@ -48,46 +47,43 @@
     <t>Giá</t>
   </si>
   <si>
-    <t>Zenbook Fold</t>
-  </si>
-  <si>
-    <t>Zenbook Duo</t>
-  </si>
-  <si>
-    <t>Zenbook Vivobook AMOLED</t>
-  </si>
-  <si>
-    <t>Alienware M15</t>
-  </si>
-  <si>
-    <t>XPS 13 Pro</t>
-  </si>
-  <si>
-    <t>Macbook Pro 14"</t>
-  </si>
-  <si>
-    <t>Macbook Mini M1</t>
-  </si>
-  <si>
-    <t>iMac 24"</t>
-  </si>
-  <si>
     <t>Hiệu</t>
   </si>
   <si>
-    <t>Asus</t>
-  </si>
-  <si>
     <t>Số lượng</t>
   </si>
   <si>
     <t>Img</t>
   </si>
   <si>
-    <t>Dell</t>
-  </si>
-  <si>
-    <t>Apple</t>
+    <t>HP Pavilion 14</t>
+  </si>
+  <si>
+    <t>/Images/hp_pavilion_14.jpg</t>
+  </si>
+  <si>
+    <t>/Images/hp15_ryzen.jpg</t>
+  </si>
+  <si>
+    <t>HP 15 Ryzen</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>/Images/msi_gf63.jpg</t>
+  </si>
+  <si>
+    <t>/Images/msi_pulse_gl66.jpg</t>
+  </si>
+  <si>
+    <t>MSI GF63</t>
+  </si>
+  <si>
+    <t>MSI Pulse GL66</t>
+  </si>
+  <si>
+    <t>MSI</t>
   </si>
 </sst>
 </file>
@@ -439,14 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447BA455-4EAE-4393-9D69-35ED214A2375}">
-  <dimension ref="B3:G6"/>
+  <dimension ref="B3:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -456,33 +453,36 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>50000000</v>
+        <v>16000000</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -492,33 +492,19 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>80000000</v>
+        <v>22000000</v>
       </c>
       <c r="G5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>24000000</v>
-      </c>
-      <c r="G6">
         <v>100</v>
       </c>
     </row>
@@ -531,13 +517,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0B9511-AD32-40E9-96AE-F3C70FB6EFAE}">
   <dimension ref="B3:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -548,33 +534,36 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4">
-        <v>14000000</v>
+        <v>20000000</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -584,107 +573,19 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5">
-        <v>15000000</v>
+        <v>17000000</v>
       </c>
       <c r="G5">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612E87DA-204E-494A-BE8F-646078C5A067}">
-  <dimension ref="B3:G6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4">
-        <v>45000000</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5">
-        <v>33000000</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>33000000</v>
-      </c>
-      <c r="G6">
         <v>100</v>
       </c>
     </row>

</xml_diff>